<commit_message>
Folhas para os dois mapas
</commit_message>
<xml_diff>
--- a/Testes.xlsx
+++ b/Testes.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jgmfe\Documents\GitHub\Projeto-IAA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Documents\GitHub\Projeto-IAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{178471B0-323B-4337-B694-24885FF784B9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF43DC6-D902-4FFF-97BF-68F8B5077F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Folha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mapa2a" sheetId="2" r:id="rId1"/>
+    <sheet name="Mapa2b" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
   <si>
     <t>Mapa2a</t>
   </si>
@@ -88,6 +89,9 @@
   </si>
   <si>
     <t>Recursos apanhados</t>
+  </si>
+  <si>
+    <t>Mapa2b</t>
   </si>
 </sst>
 </file>
@@ -405,7 +409,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A668E9B-DE86-4C52-857A-ECF2AD6B7CB4}">
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -596,4 +600,200 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:W14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="1"/>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+      <c r="T4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" t="s">
+        <v>6</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
+        <v>9</v>
+      </c>
+      <c r="P5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>11</v>
+      </c>
+      <c r="R5" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" t="s">
+        <v>13</v>
+      </c>
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5" t="s">
+        <v>17</v>
+      </c>
+      <c r="V5" t="s">
+        <v>20</v>
+      </c>
+      <c r="W5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="K7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="K12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="K13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update codigo e testes
</commit_message>
<xml_diff>
--- a/Testes.xlsx
+++ b/Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Documents\GitHub\Projeto-IAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF43DC6-D902-4FFF-97BF-68F8B5077F96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77AB3ED-360E-44DF-81A5-CB6636ED6FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="29">
   <si>
     <t>Mapa2a</t>
   </si>
@@ -92,6 +92,27 @@
   </si>
   <si>
     <t>Mapa2b</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>Não</t>
+  </si>
+  <si>
+    <t>Sim, no fim do mapa</t>
+  </si>
+  <si>
+    <t>0-2,3</t>
+  </si>
+  <si>
+    <t>Strenght Factor</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
+  <si>
+    <t>0-0,3</t>
   </si>
 </sst>
 </file>
@@ -412,7 +433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A668E9B-DE86-4C52-857A-ECF2AD6B7CB4}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -429,6 +452,7 @@
     <col min="12" max="12" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" customWidth="1"/>
     <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="10.88671875" bestFit="1" customWidth="1"/>
@@ -499,6 +523,9 @@
       <c r="N5" t="s">
         <v>9</v>
       </c>
+      <c r="O5" t="s">
+        <v>26</v>
+      </c>
       <c r="P5" t="s">
         <v>10</v>
       </c>
@@ -576,24 +603,186 @@
       <c r="A12" t="s">
         <v>5</v>
       </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12">
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>22</v>
+      </c>
       <c r="K12" t="s">
         <v>3</v>
+      </c>
+      <c r="L12">
+        <v>5</v>
+      </c>
+      <c r="M12">
+        <v>90</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12" t="s">
+        <v>22</v>
+      </c>
+      <c r="S12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" t="s">
+        <v>23</v>
+      </c>
+      <c r="U12" t="s">
+        <v>24</v>
+      </c>
+      <c r="V12">
+        <v>1</v>
+      </c>
+      <c r="W12">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>22</v>
+      </c>
       <c r="K13" t="s">
         <v>4</v>
+      </c>
+      <c r="L13">
+        <v>5</v>
+      </c>
+      <c r="M13">
+        <v>90</v>
+      </c>
+      <c r="N13">
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>5</v>
       </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>22</v>
+      </c>
       <c r="K14" t="s">
         <v>5</v>
+      </c>
+      <c r="L14">
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <v>90</v>
+      </c>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="O14">
+        <v>0.02</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" t="s">
+        <v>25</v>
+      </c>
+      <c r="T14" t="s">
+        <v>27</v>
+      </c>
+      <c r="U14" t="s">
+        <v>23</v>
+      </c>
+      <c r="V14">
+        <v>1</v>
+      </c>
+      <c r="W14">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Funcao Gaussiana corrigida e testes
</commit_message>
<xml_diff>
--- a/Testes.xlsx
+++ b/Testes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Documents\GitHub\Projeto-IAA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A77AB3ED-360E-44DF-81A5-CB6636ED6FB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8391CDA4-9354-42C6-83DB-DAB7C59F433A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="31">
   <si>
     <t>Mapa2a</t>
   </si>
@@ -113,6 +113,12 @@
   </si>
   <si>
     <t>0-0,3</t>
+  </si>
+  <si>
+    <t>0,1-0,7</t>
+  </si>
+  <si>
+    <t>0-3</t>
   </si>
 </sst>
 </file>
@@ -434,7 +440,7 @@
   <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S15" sqref="S15"/>
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -712,6 +718,33 @@
       </c>
       <c r="N13">
         <v>10</v>
+      </c>
+      <c r="O13">
+        <v>0.01</v>
+      </c>
+      <c r="P13">
+        <v>0.2</v>
+      </c>
+      <c r="Q13">
+        <v>0.04</v>
+      </c>
+      <c r="R13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S13" t="s">
+        <v>30</v>
+      </c>
+      <c r="T13" t="s">
+        <v>27</v>
+      </c>
+      <c r="U13" t="s">
+        <v>23</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>